<commit_message>
add CPU memory table
</commit_message>
<xml_diff>
--- a/Summary/CompareResult.xlsx
+++ b/Summary/CompareResult.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sam/Desktop/D/CMU/Course/18845_Internet_Service/final_project/serverless-study/Figure_Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sam/Desktop/D/CMU/Course/18845_Internet_Service/final_project/serverless-study/Summary/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
     <sheet name="LightCPU_Memory" sheetId="4" r:id="rId4"/>
     <sheet name="HeavyCPU_Memory" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="39">
   <si>
     <t>StarTime</t>
   </si>
@@ -130,6 +130,54 @@
     <t>Function number 7</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>max memory usage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Max memory usage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clofly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenLambda</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light Load Max Memory Usage (MB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Heavy Load Max Memory Usage (MB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>max usage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duration (seconds)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average CPU idle (%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU average</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min CPU idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -164,6 +212,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="新細明體"/>
+      <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -203,22 +252,35 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1286,11 +1348,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-497799152"/>
-        <c:axId val="-402755440"/>
+        <c:axId val="-405003472"/>
+        <c:axId val="-404027824"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-497799152"/>
+        <c:axId val="-405003472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,7 +1411,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-402755440"/>
+        <c:crossAx val="-404027824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1358,7 +1420,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-402755440"/>
+        <c:axId val="-404027824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1398,7 +1460,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -1419,7 +1480,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-497799152"/>
+        <c:crossAx val="-405003472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2717,11 +2778,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-318819168"/>
-        <c:axId val="-266643616"/>
+        <c:axId val="-265252208"/>
+        <c:axId val="-265249360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-318819168"/>
+        <c:axId val="-265252208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2776,7 +2837,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-266643616"/>
+        <c:crossAx val="-265249360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2786,7 +2847,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-266643616"/>
+        <c:axId val="-265249360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,7 +2914,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-318819168"/>
+        <c:crossAx val="-265252208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3306,11 +3367,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-366127280"/>
-        <c:axId val="-363167408"/>
+        <c:axId val="-265033408"/>
+        <c:axId val="-265030016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-366127280"/>
+        <c:axId val="-265033408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="21.0"/>
@@ -3342,7 +3403,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3366,7 +3426,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-363167408"/>
+        <c:crossAx val="-265030016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -3376,7 +3436,7 @@
         <c:minorUnit val="1.0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-363167408"/>
+        <c:axId val="-265030016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3416,7 +3476,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -3437,7 +3496,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-366127280"/>
+        <c:crossAx val="-265033408"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3889,11 +3948,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-325825648"/>
-        <c:axId val="-289270368"/>
+        <c:axId val="-459235424"/>
+        <c:axId val="-403350480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-325825648"/>
+        <c:axId val="-459235424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.0"/>
@@ -3925,7 +3984,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3949,7 +4007,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-289270368"/>
+        <c:crossAx val="-403350480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -3959,7 +4017,7 @@
         <c:minorUnit val="1.0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-289270368"/>
+        <c:axId val="-403350480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3990,7 +4048,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4011,7 +4068,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-325825648"/>
+        <c:crossAx val="-459235424"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4460,11 +4517,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-326897152"/>
-        <c:axId val="-285505408"/>
+        <c:axId val="-403117968"/>
+        <c:axId val="-403412704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-326897152"/>
+        <c:axId val="-403117968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.0"/>
@@ -4496,7 +4553,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4520,7 +4576,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-285505408"/>
+        <c:crossAx val="-403412704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -4530,7 +4586,7 @@
         <c:minorUnit val="1.0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-285505408"/>
+        <c:axId val="-403412704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4561,7 +4617,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4582,7 +4637,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326897152"/>
+        <c:crossAx val="-403117968"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5034,11 +5089,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-288211136"/>
-        <c:axId val="-289278624"/>
+        <c:axId val="-403449824"/>
+        <c:axId val="-265021536"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-288211136"/>
+        <c:axId val="-403449824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.0"/>
@@ -5070,7 +5125,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5094,7 +5148,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-289278624"/>
+        <c:crossAx val="-265021536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -5104,7 +5158,7 @@
         <c:minorUnit val="1.0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-289278624"/>
+        <c:axId val="-265021536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5135,7 +5189,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5156,7 +5209,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-288211136"/>
+        <c:crossAx val="-403449824"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5578,11 +5631,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-362437760"/>
-        <c:axId val="-325598208"/>
+        <c:axId val="-265088048"/>
+        <c:axId val="-265084656"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-362437760"/>
+        <c:axId val="-265088048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.0"/>
@@ -5614,7 +5667,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -5638,7 +5690,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-325598208"/>
+        <c:crossAx val="-265084656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -5648,7 +5700,7 @@
         <c:minorUnit val="1.0"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-325598208"/>
+        <c:axId val="-265084656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5679,7 +5731,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -5700,7 +5751,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-362437760"/>
+        <c:crossAx val="-265088048"/>
         <c:crossesAt val="1.0"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6998,11 +7049,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-285344496"/>
-        <c:axId val="-321222080"/>
+        <c:axId val="-264920480"/>
+        <c:axId val="-264917088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-285344496"/>
+        <c:axId val="-264920480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7057,7 +7108,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-321222080"/>
+        <c:crossAx val="-264917088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7067,7 +7118,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-321222080"/>
+        <c:axId val="-264917088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -7128,7 +7179,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-285344496"/>
+        <c:crossAx val="-264920480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8426,11 +8477,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-459512032"/>
-        <c:axId val="-459509840"/>
+        <c:axId val="-264883344"/>
+        <c:axId val="-264879952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-459512032"/>
+        <c:axId val="-264883344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8485,7 +8536,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-459509840"/>
+        <c:crossAx val="-264879952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8495,7 +8546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-459509840"/>
+        <c:axId val="-264879952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200.0"/>
@@ -8563,7 +8614,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-459512032"/>
+        <c:crossAx val="-264883344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9861,11 +9912,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-326310896"/>
-        <c:axId val="-326941456"/>
+        <c:axId val="-264929440"/>
+        <c:axId val="-264961488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-326310896"/>
+        <c:axId val="-264929440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9920,7 +9971,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326941456"/>
+        <c:crossAx val="-264961488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9930,7 +9981,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-326941456"/>
+        <c:axId val="-264961488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100.0"/>
@@ -9991,7 +10042,7 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-326310896"/>
+        <c:crossAx val="-264929440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10245,13 +10296,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>491628</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>1497</xdr:rowOff>
@@ -10277,13 +10328,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>491628</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>1497</xdr:rowOff>
@@ -26058,15 +26109,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:AH62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O7" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="AB28" sqref="AB28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
+      <selection activeCell="AE8" sqref="AE8:AH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="32" max="32" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="22.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -26080,7 +26136,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -26096,6 +26152,9 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
       <c r="H2" t="s">
         <v>17</v>
       </c>
@@ -26111,6 +26170,9 @@
       <c r="L2" t="s">
         <v>25</v>
       </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
       <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
@@ -26126,8 +26188,17 @@
       <c r="S2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1492742120.974</v>
       </c>
@@ -26145,6 +26216,10 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="F3">
+        <f>MAX(D3:D62)</f>
+        <v>572.40234375</v>
+      </c>
       <c r="H3">
         <v>1492741647.473</v>
       </c>
@@ -26162,6 +26237,10 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="M3">
+        <f>MAX(K3:K4)</f>
+        <v>732.9140625</v>
+      </c>
       <c r="O3">
         <v>1492741493.3069999</v>
       </c>
@@ -26178,8 +26257,22 @@
       <c r="S3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T3">
+        <f>MAX(R3:R62)</f>
+        <v>784.88671875</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3">
+        <f>F3</f>
+        <v>572.40234375</v>
+      </c>
+      <c r="AG3">
+        <v>583.44921875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1492742121.9749999</v>
       </c>
@@ -26231,8 +26324,18 @@
         <f>O4-$O$3</f>
         <v>1.0010001659393311</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="AE4" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF4">
+        <f>M3</f>
+        <v>732.9140625</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>953.3671875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1492742122.9749999</v>
       </c>
@@ -26250,6 +26353,9 @@
         <f t="shared" ref="E5:E62" si="3">A5-$A$3</f>
         <v>2.000999927520752</v>
       </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
       <c r="H5">
         <v>1492741649.474</v>
       </c>
@@ -26267,6 +26373,9 @@
         <f t="shared" ref="L5:L62" si="4">H5-$H$3</f>
         <v>2.000999927520752</v>
       </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
       <c r="O5">
         <v>1492741495.3080001</v>
       </c>
@@ -26284,8 +26393,21 @@
         <f>O5-$O$3</f>
         <v>2.0010001659393311</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF5">
+        <f>T3</f>
+        <v>784.88671875</v>
+      </c>
+      <c r="AG5">
+        <v>843.12109375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1492742123.9749999</v>
       </c>
@@ -26303,6 +26425,10 @@
         <f t="shared" si="3"/>
         <v>3.000999927520752</v>
       </c>
+      <c r="F6">
+        <f>MIN(B8:B37)</f>
+        <v>22</v>
+      </c>
       <c r="H6">
         <v>1492741650.474</v>
       </c>
@@ -26320,6 +26446,10 @@
         <f t="shared" si="4"/>
         <v>3.000999927520752</v>
       </c>
+      <c r="M6">
+        <f>MIN(I10:I35)</f>
+        <v>0</v>
+      </c>
       <c r="O6">
         <v>1492741496.3080001</v>
       </c>
@@ -26337,8 +26467,12 @@
         <f t="shared" ref="S6:S62" si="5">O6-$O$3</f>
         <v>3.0010001659393311</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T6">
+        <f>MIN(P8:P10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1492742124.9749999</v>
       </c>
@@ -26391,7 +26525,7 @@
         <v>4.0010001659393311</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1492742125.9749999</v>
       </c>
@@ -26409,6 +26543,9 @@
         <f t="shared" si="3"/>
         <v>5.000999927520752</v>
       </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
       <c r="H8">
         <v>1492741652.474</v>
       </c>
@@ -26426,6 +26563,9 @@
         <f t="shared" si="4"/>
         <v>5.000999927520752</v>
       </c>
+      <c r="M8" t="s">
+        <v>37</v>
+      </c>
       <c r="O8">
         <v>1492741498.3080001</v>
       </c>
@@ -26443,8 +26583,20 @@
         <f t="shared" si="5"/>
         <v>5.0010001659393311</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1492742126.9749999</v>
       </c>
@@ -26462,6 +26614,10 @@
         <f t="shared" si="3"/>
         <v>6.000999927520752</v>
       </c>
+      <c r="F9">
+        <f>AVERAGE(B8:B37)</f>
+        <v>29.203066666666665</v>
+      </c>
       <c r="H9">
         <v>1492741653.474</v>
       </c>
@@ -26479,6 +26635,10 @@
         <f t="shared" si="4"/>
         <v>6.000999927520752</v>
       </c>
+      <c r="M9">
+        <f>AVERAGE(I10:I35)</f>
+        <v>12.654500000000001</v>
+      </c>
       <c r="O9">
         <v>1492741499.3080001</v>
       </c>
@@ -26496,8 +26656,24 @@
         <f t="shared" si="5"/>
         <v>6.0010001659393311</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T9">
+        <f>AVERAGE(P8:P10)</f>
+        <v>24.192666666666668</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF9">
+        <v>30</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="AH9" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1492742127.9749999</v>
       </c>
@@ -26549,8 +26725,20 @@
         <f t="shared" si="5"/>
         <v>7.0010001659393311</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="AE10" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF10">
+        <v>26</v>
+      </c>
+      <c r="AG10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH10" s="5">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1492742128.9749999</v>
       </c>
@@ -26602,8 +26790,20 @@
         <f t="shared" si="5"/>
         <v>8.0010001659393311</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="AE11" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF11">
+        <v>4</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="5">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1492742129.9749999</v>
       </c>
@@ -26656,7 +26856,7 @@
         <v>9.0010001659393311</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1492742130.9749999</v>
       </c>
@@ -26709,7 +26909,7 @@
         <v>10.001000165939331</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1492742131.9749999</v>
       </c>
@@ -26762,7 +26962,7 @@
         <v>11.001000165939331</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1492742132.9749999</v>
       </c>
@@ -26815,7 +27015,7 @@
         <v>12.001000165939331</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1492742133.9749999</v>
       </c>
@@ -29315,15 +29515,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView topLeftCell="S13" zoomScale="139" workbookViewId="0">
-      <selection activeCell="AD27" sqref="AD27"/>
+    <sheetView topLeftCell="S1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="AD15" sqref="AD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -29337,7 +29537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -29353,6 +29553,9 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
       <c r="H2" t="s">
         <v>17</v>
       </c>
@@ -29368,6 +29571,9 @@
       <c r="L2" t="s">
         <v>25</v>
       </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
       <c r="O2" s="1" t="s">
         <v>17</v>
       </c>
@@ -29383,8 +29589,11 @@
       <c r="S2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1492742270.9809999</v>
       </c>
@@ -29402,6 +29611,10 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="F3">
+        <f>MAX(D3:D62)</f>
+        <v>583.44921875</v>
+      </c>
       <c r="H3">
         <v>1492741797.4790001</v>
       </c>
@@ -29419,6 +29632,10 @@
         <f>0</f>
         <v>0</v>
       </c>
+      <c r="M3">
+        <f>MAX(K3:K62)</f>
+        <v>953.3671875</v>
+      </c>
       <c r="O3">
         <v>1492741643.3150001</v>
       </c>
@@ -29435,8 +29652,12 @@
       <c r="S3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="T3">
+        <f>MAX(R3:R62)</f>
+        <v>843.12109375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1492742271.983</v>
       </c>
@@ -29489,7 +29710,7 @@
         <v>1.000999927520752</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>1492742272.983</v>
       </c>
@@ -29542,7 +29763,7 @@
         <v>2.000999927520752</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>1492742273.983</v>
       </c>
@@ -29595,7 +29816,7 @@
         <v>3.000999927520752</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>1492742274.983</v>
       </c>
@@ -29648,7 +29869,7 @@
         <v>4.000999927520752</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>1492742275.9820001</v>
       </c>
@@ -29701,7 +29922,7 @@
         <v>5.000999927520752</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>1492742276.9820001</v>
       </c>
@@ -29754,7 +29975,7 @@
         <v>6.000999927520752</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>1492742277.9820001</v>
       </c>
@@ -29807,7 +30028,7 @@
         <v>7.000999927520752</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>1492742278.983</v>
       </c>
@@ -29860,7 +30081,7 @@
         <v>8.000999927520752</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>1492742279.9820001</v>
       </c>
@@ -29913,7 +30134,7 @@
         <v>9.000999927520752</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>1492742280.9820001</v>
       </c>
@@ -29966,7 +30187,7 @@
         <v>10.000999927520752</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>1492742281.9820001</v>
       </c>
@@ -30019,7 +30240,7 @@
         <v>11.000999927520752</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1492742282.9820001</v>
       </c>
@@ -30072,7 +30293,7 @@
         <v>12.000999927520752</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>1492742283.983</v>
       </c>

</xml_diff>